<commit_message>
# Please enter the commit message for your changes. Lines starting # with '#' will be ignored, and an empty message aborts the commit. # # On branch main # Your branch is up to date with 'origin/main'. # # Changes to be committed: #	modified:   database/caminhoes_frota.xlsx #	modified:   database/coordenadas_salvas.xlsx #
</commit_message>
<xml_diff>
--- a/database/caminhoes_frota.xlsx
+++ b/database/caminhoes_frota.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:F82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2705,6 +2705,18 @@
         </is>
       </c>
     </row>
+    <row r="82">
+      <c r="A82" t="inlineStr"/>
+      <c r="B82" t="inlineStr"/>
+      <c r="C82" t="inlineStr"/>
+      <c r="D82" t="inlineStr"/>
+      <c r="E82" t="inlineStr"/>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>